<commit_message>
Adding test cases related to ISP order. Warning removed.
</commit_message>
<xml_diff>
--- a/resources/testdata/OrderIspBCT.xlsx
+++ b/resources/testdata/OrderIspBCT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>TCID</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>TestForOrderProvisioned</t>
-  </si>
-  <si>
-    <t>password</t>
   </si>
   <si>
     <t>purchesOrderNo</t>
@@ -489,34 +486,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding order related test cases.
</commit_message>
<xml_diff>
--- a/resources/testdata/OrderIspBCT.xlsx
+++ b/resources/testdata/OrderIspBCT.xlsx
@@ -8,15 +8,25 @@
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
-    <sheet name="TestForOrderProvisioned" sheetId="4" r:id="rId2"/>
-    <sheet name="placeOrder" sheetId="3" r:id="rId3"/>
+    <sheet name="verifyOrderCancel" sheetId="14" r:id="rId2"/>
+    <sheet name="cancelOrder" sheetId="13" r:id="rId3"/>
+    <sheet name="verifyOrderDowngraded" sheetId="12" r:id="rId4"/>
+    <sheet name="downgradeOrder" sheetId="11" r:id="rId5"/>
+    <sheet name="verifyOrderUpgraded" sheetId="10" r:id="rId6"/>
+    <sheet name="upgradeOrder" sheetId="9" r:id="rId7"/>
+    <sheet name="verifyOrderDownsized" sheetId="8" r:id="rId8"/>
+    <sheet name="downsizeOrder" sheetId="7" r:id="rId9"/>
+    <sheet name="verifyOrderUpsized" sheetId="6" r:id="rId10"/>
+    <sheet name="upsizeOrder" sheetId="5" r:id="rId11"/>
+    <sheet name="placeOrder" sheetId="3" r:id="rId12"/>
+    <sheet name="verifyOrderProvisioned" sheetId="4" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>TCID</t>
   </si>
@@ -66,9 +76,6 @@
     <t>placeOrder</t>
   </si>
   <si>
-    <t>autoIspOrderOrg</t>
-  </si>
-  <si>
     <t>MyCloud Service</t>
   </si>
   <si>
@@ -78,16 +85,73 @@
     <t>{"ItemList":[{"itemName":"Disk Quota1","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"User Quota1","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"5"},{"itemName":"Disk Quota PPU1","operation":"True","textbox":"False","dropdown":"False","checkbox":"True","value":"0"},{"itemName":"User Quota PPU1","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"2"},{"itemName":"User Quota2","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"30.0"},{"itemName":"Disk Quota2","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"2"}]}</t>
   </si>
   <si>
-    <t>{"ProvInfoLst":[{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Organization Name *","textbox":"True","value":"Sample Test Org"},{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Domain Name","textbox":"True","value":"mytestdomain.isp"},{"checkbox":"True","dropdown":"False","operation":"True","provInfoName":"BooleanType","textbox":"False","value":"pratap@domain.com"},{"checkbox":"False","dropdown":"True","operation":"True","provInfoName":"PrivateDomainName","textbox":"False","value":"dom1001.isp"},{"checkbox":"False","dropdown":"True","operation":"True","provInfoName":"List of values","textbox":"False","value":"DisplayName1"},{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Purchase Order Number","textbox":"True","value":"isp-abc-fgtd-dcrt-tfdtc-asdef"},{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Custom Field1 *","textbox":"True","value":"xyz"}    ] }</t>
-  </si>
-  <si>
-    <t>TestForOrderProvisioned</t>
-  </si>
-  <si>
     <t>purchesOrderNo</t>
   </si>
   <si>
-    <t>isp-abc-fgtd-dcrt-tfdtc-asdef</t>
+    <t>verifyOrderProvisioned</t>
+  </si>
+  <si>
+    <t>upsizeOrder</t>
+  </si>
+  <si>
+    <t>verifyOrderUpsized</t>
+  </si>
+  <si>
+    <t>downsizeOrder</t>
+  </si>
+  <si>
+    <t>verifyOrderDownsized</t>
+  </si>
+  <si>
+    <t>upgradeOrder</t>
+  </si>
+  <si>
+    <t>verifyOrderUpgraded</t>
+  </si>
+  <si>
+    <t>downgradeOrder</t>
+  </si>
+  <si>
+    <t>verifyOrderDowngraded</t>
+  </si>
+  <si>
+    <t>cancelOrder</t>
+  </si>
+  <si>
+    <t>verifyOrderCancel</t>
+  </si>
+  <si>
+    <t>demo Test</t>
+  </si>
+  <si>
+    <t>{"ProvInfoLst":[{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Organization Name *","textbox":"True","value":"Sample Test Org"},{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Domain Name","textbox":"True","value":"mytestdomain.isp"},{"checkbox":"True","dropdown":"False","operation":"True","provInfoName":"BooleanType","textbox":"False","value":"pratap@domain.com"},{"checkbox":"False","dropdown":"True","operation":"True","provInfoName":"PrivateDomainName","textbox":"False","value":"pratapadsync.com"},{"checkbox":"False","dropdown":"True","operation":"True","provInfoName":"List of values","textbox":"False","value":"DisplayName1"},{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Purchase Order Number","textbox":"True","value":"isp-abc-fgtd-dcrt-tfdtc"},{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Custom Field1 *","textbox":"True","value":"xyz"}    ] }</t>
+  </si>
+  <si>
+    <t>isp-abc-fgtd-dcrt-tfdtc</t>
+  </si>
+  <si>
+    <t>{"ItemList":[{"itemName":"Disk Quota1","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"User Quota1","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"8"},{"itemName":"Disk Quota PPU1","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"User Quota PPU1","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"7"},{"itemName":"User Quota2","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"40.0"},{"itemName":"Disk Quota2","operation":"False","textbox":"True","dropdown":"False","checkbox":"False","value":"2"}]}</t>
+  </si>
+  <si>
+    <t>{"ItemList":[{"itemName":"Disk Quota1","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"User Quota1","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"4"},{"itemName":"Disk Quota PPU1","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"User Quota PPU1","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"7"},{"itemName":"User Quota2","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"30.0"},{"itemName":"Disk Quota2","operation":"False","textbox":"True","dropdown":"False","checkbox":"False","value":"2"}]}</t>
+  </si>
+  <si>
+    <t>upgradeOfferName</t>
+  </si>
+  <si>
+    <t>MyCloud Offer to upgrade</t>
+  </si>
+  <si>
+    <t>{"ProvInfoLst":[{"provInfoName":"BooleanType","operation":"True","textbox":"False","dropdown":"False","checkbox":"True","value":"pratap@domain.com"},{"provInfoName":"List of values","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"DisplayName2"},{"provInfoName":"Custom Field3","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"xyz2"}]}</t>
+  </si>
+  <si>
+    <t>downgradeOfferName</t>
+  </si>
+  <si>
+    <t>MyCloud Offer To Down</t>
+  </si>
+  <si>
+    <t>{"ProvInfoLst":[{"provInfoName":"BooleanType","operation":"True","textbox":"False","dropdown":"False","checkbox":"True","value":"pratap@domain.com"},{"provInfoName":"List of values","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"DisplayName3"},{"provInfoName":"Custom Field4","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"xyz3"}]}</t>
   </si>
 </sst>
 </file>
@@ -436,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,51 +537,139 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -553,22 +705,301 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2">
+        <v>10046</v>
+      </c>
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
-        <v>20</v>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated for running ISP on 86 server
</commit_message>
<xml_diff>
--- a/resources/testdata/OrderIspBCT.xlsx
+++ b/resources/testdata/OrderIspBCT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>TCID</t>
   </si>
@@ -76,9 +76,6 @@
     <t>placeOrder</t>
   </si>
   <si>
-    <t>MyCloud Service</t>
-  </si>
-  <si>
     <t>MyCloud Offer</t>
   </si>
   <si>
@@ -121,12 +118,6 @@
     <t>verifyOrderCancel</t>
   </si>
   <si>
-    <t>demo Test</t>
-  </si>
-  <si>
-    <t>{"ProvInfoLst":[{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Organization Name *","textbox":"True","value":"Sample Test Org"},{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Domain Name","textbox":"True","value":"mytestdomain.isp"},{"checkbox":"True","dropdown":"False","operation":"True","provInfoName":"BooleanType","textbox":"False","value":"pratap@domain.com"},{"checkbox":"False","dropdown":"True","operation":"True","provInfoName":"PrivateDomainName","textbox":"False","value":"pratapadsync.com"},{"checkbox":"False","dropdown":"True","operation":"True","provInfoName":"List of values","textbox":"False","value":"DisplayName1"},{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Purchase Order Number","textbox":"True","value":"isp-abc-fgtd-dcrt-tfdtc"},{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Custom Field1 *","textbox":"True","value":"xyz"}    ] }</t>
-  </si>
-  <si>
     <t>isp-abc-fgtd-dcrt-tfdtc</t>
   </si>
   <si>
@@ -139,19 +130,31 @@
     <t>upgradeOfferName</t>
   </si>
   <si>
-    <t>MyCloud Offer to upgrade</t>
-  </si>
-  <si>
     <t>{"ProvInfoLst":[{"provInfoName":"BooleanType","operation":"True","textbox":"False","dropdown":"False","checkbox":"True","value":"pratap@domain.com"},{"provInfoName":"List of values","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"DisplayName2"},{"provInfoName":"Custom Field3","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"xyz2"}]}</t>
   </si>
   <si>
     <t>downgradeOfferName</t>
   </si>
   <si>
-    <t>MyCloud Offer To Down</t>
-  </si>
-  <si>
     <t>{"ProvInfoLst":[{"provInfoName":"BooleanType","operation":"True","textbox":"False","dropdown":"False","checkbox":"True","value":"pratap@domain.com"},{"provInfoName":"List of values","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"DisplayName3"},{"provInfoName":"Custom Field4","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"xyz3"}]}</t>
+  </si>
+  <si>
+    <t>isp-abc-fgtd-dcrt-tfdqa</t>
+  </si>
+  <si>
+    <t>Order BCT ISP</t>
+  </si>
+  <si>
+    <t>My Cloud</t>
+  </si>
+  <si>
+    <t>{"ProvInfoLst":[{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Organization Name *","textbox":"True","value":"Sample Test Org"},{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Domain Name","textbox":"True","value":"mytestdomain.isp"},{"checkbox":"True","dropdown":"False","operation":"True","provInfoName":"BooleanType","textbox":"False","value":"pratap@domain.com"},{"checkbox":"False","dropdown":"True","operation":"True","provInfoName":"PrivateDomainName","textbox":"False","value":"orderbctisp.com"},{"checkbox":"False","dropdown":"True","operation":"True","provInfoName":"List of values","textbox":"False","value":"DisplayName1"},{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Purchase Order Number","textbox":"True","value":"isp-abc-fgtd-dcrt-tfdqa"},{"checkbox":"False","dropdown":"False","operation":"True","provInfoName":"Custom Field2 *","textbox":"True","value":"xyz"}    ] }</t>
+  </si>
+  <si>
+    <t>MyCloud Offer To Upgrade</t>
+  </si>
+  <si>
+    <t>MyCloud Offer To Downgrade</t>
   </si>
 </sst>
 </file>
@@ -537,7 +540,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -545,52 +548,52 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -613,12 +616,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -646,7 +649,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -658,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,30 +708,58 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2">
+        <v>10015</v>
+      </c>
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="F2">
-        <v>10046</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -738,99 +769,73 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -843,7 +848,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +860,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -866,41 +871,41 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -913,7 +918,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,7 +930,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -936,22 +941,50 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -961,45 +994,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>